<commit_message>
PSNR/DOWNSCALE: Opdateret i LC, Main og OT, tjek beskrivelse
OT, main og LC: PSNR kører på checkerboards fremfor hele billeder.
OT: Justeret Excel kun med nødvendige ting.
LC: Opdateret til at scale down fremfor upscale
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Spinat/Spinach20g/Results/OTResults.xlsx
+++ b/P3/Results/Data/Spinat/Spinach20g/Results/OTResults.xlsx
@@ -412,13 +412,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="44" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -428,77 +440,47 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Psnr Ground diff Reference</t>
+          <t>PSNR Ground checker diff Reference checker</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Psnr Ground diff Enhanced</t>
+          <t>PSNR Ground checker diff Enhanced checker</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Psnr Reference diff Enhanced</t>
+          <t>MBE Ground diff Reference</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Psnr Ground diff Dehazed</t>
+          <t>MBE Ground diff Enhanced</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Psnr Reference diff Dehazed</t>
+          <t>MBE Ground diff Dehazed</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>MBE Ground diff Reference</t>
+          <t>AG Ground</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>MBE Ground diff Enhanced</t>
+          <t>AG Reference</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>MBE Reference diff Enhanced</t>
+          <t>AG Enhanced</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>MBE Ground diff Dehazed</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>MBE Reference diff Dehazed</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>AG Ground diff Reference</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>AG Ground diff Enhanced</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>AG Reference diff Enhanced</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>AG Ground diff Dehazed</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>AG Reference diff Dehazed</t>
+          <t>AG Dehazed</t>
         </is>
       </c>
     </row>
@@ -509,49 +491,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16.34</v>
+        <v>8.57</v>
       </c>
       <c r="C2" t="n">
-        <v>14.57</v>
+        <v>10.01</v>
       </c>
       <c r="D2" t="n">
-        <v>20.75</v>
+        <v>6.07</v>
       </c>
       <c r="E2" t="n">
-        <v>15.15</v>
+        <v>19.83</v>
       </c>
       <c r="F2" t="n">
-        <v>23.22</v>
+        <v>20.21</v>
       </c>
       <c r="G2" t="n">
-        <v>6.07</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>19.8</v>
+        <v>4.77</v>
       </c>
       <c r="I2" t="n">
-        <v>13.73</v>
+        <v>24.03</v>
       </c>
       <c r="J2" t="n">
-        <v>20.21</v>
-      </c>
-      <c r="K2" t="n">
-        <v>14.14</v>
-      </c>
-      <c r="L2" t="n">
-        <v>3.85</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-15.44</v>
-      </c>
-      <c r="N2" t="n">
-        <v>-19.29</v>
-      </c>
-      <c r="O2" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="P2" t="n">
-        <v>-0.77</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="3">
@@ -561,49 +525,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16.2</v>
+        <v>7.27</v>
       </c>
       <c r="C3" t="n">
-        <v>14.22</v>
+        <v>8.85</v>
       </c>
       <c r="D3" t="n">
-        <v>19.97</v>
+        <v>13.03</v>
       </c>
       <c r="E3" t="n">
-        <v>15.16</v>
+        <v>17.27</v>
       </c>
       <c r="F3" t="n">
-        <v>27.1</v>
+        <v>22.58</v>
       </c>
       <c r="G3" t="n">
-        <v>13.03</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>17.27</v>
+        <v>3.42</v>
       </c>
       <c r="I3" t="n">
-        <v>4.24</v>
+        <v>30.44</v>
       </c>
       <c r="J3" t="n">
-        <v>22.58</v>
-      </c>
-      <c r="K3" t="n">
-        <v>9.550000000000001</v>
-      </c>
-      <c r="L3" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-21.99</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-27.19</v>
-      </c>
-      <c r="O3" t="n">
-        <v>4.51</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-0.6899999999999999</v>
+        <v>4.11</v>
       </c>
     </row>
     <row r="4">
@@ -613,49 +559,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16.67</v>
+        <v>8.77</v>
       </c>
       <c r="C4" t="n">
-        <v>15.39</v>
+        <v>6.98</v>
       </c>
       <c r="D4" t="n">
-        <v>19.37</v>
+        <v>-3.96</v>
       </c>
       <c r="E4" t="n">
-        <v>15.45</v>
+        <v>19.51</v>
       </c>
       <c r="F4" t="n">
-        <v>19.15</v>
+        <v>18.49</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.96</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>19.52</v>
+        <v>7.92</v>
       </c>
       <c r="I4" t="n">
-        <v>23.48</v>
+        <v>12.11</v>
       </c>
       <c r="J4" t="n">
-        <v>18.49</v>
-      </c>
-      <c r="K4" t="n">
-        <v>22.45</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-3.47</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-4.17</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-0.62</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -665,49 +593,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.82</v>
+        <v>7.12</v>
       </c>
       <c r="C5" t="n">
-        <v>15.23</v>
+        <v>5.99</v>
       </c>
       <c r="D5" t="n">
-        <v>22.53</v>
+        <v>8.6</v>
       </c>
       <c r="E5" t="n">
-        <v>15.27</v>
+        <v>17.57</v>
       </c>
       <c r="F5" t="n">
-        <v>23.83</v>
+        <v>22.04</v>
       </c>
       <c r="G5" t="n">
-        <v>8.6</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>17.61</v>
+        <v>4.81</v>
       </c>
       <c r="I5" t="n">
-        <v>9.01</v>
+        <v>16.73</v>
       </c>
       <c r="J5" t="n">
-        <v>22.04</v>
-      </c>
-      <c r="K5" t="n">
-        <v>13.44</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-8.039999999999999</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-11.85</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-0.67</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="6">
@@ -717,49 +627,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15.23</v>
+        <v>11.48</v>
       </c>
       <c r="C6" t="n">
-        <v>13.27</v>
+        <v>10.17</v>
       </c>
       <c r="D6" t="n">
-        <v>20.41</v>
+        <v>-4.13</v>
       </c>
       <c r="E6" t="n">
-        <v>14.59</v>
+        <v>6.19</v>
       </c>
       <c r="F6" t="n">
-        <v>18.61</v>
+        <v>16.14</v>
       </c>
       <c r="G6" t="n">
-        <v>-4.13</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>6.21</v>
+        <v>7.73</v>
       </c>
       <c r="I6" t="n">
-        <v>10.35</v>
+        <v>13.82</v>
       </c>
       <c r="J6" t="n">
-        <v>16.14</v>
-      </c>
-      <c r="K6" t="n">
-        <v>20.27</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-5.17</v>
-      </c>
-      <c r="N6" t="n">
-        <v>-6.06</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="P6" t="n">
-        <v>-0.51</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="7">
@@ -769,49 +661,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16.33</v>
+        <v>8.74</v>
       </c>
       <c r="C7" t="n">
-        <v>13.32</v>
+        <v>10.09</v>
       </c>
       <c r="D7" t="n">
-        <v>18.02</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>15.14</v>
+        <v>4.46</v>
       </c>
       <c r="F7" t="n">
-        <v>23.7</v>
+        <v>21</v>
       </c>
       <c r="G7" t="n">
-        <v>8.539999999999999</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>4.48</v>
+        <v>4.79</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.06</v>
+        <v>16.88</v>
       </c>
       <c r="J7" t="n">
-        <v>21</v>
-      </c>
-      <c r="K7" t="n">
-        <v>12.46</v>
-      </c>
-      <c r="L7" t="n">
-        <v>3.83</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-8.26</v>
-      </c>
-      <c r="N7" t="n">
-        <v>-12.09</v>
-      </c>
-      <c r="O7" t="n">
-        <v>3.11</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-0.72</v>
+        <v>5.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>